<commit_message>
File names entered in that file name row for all excel files
</commit_message>
<xml_diff>
--- a/Automationdashboard/MAIN_FOLDER/Automation_Dashboard_Batterywise/V4/D11_03_2024/merged_analysis.xlsx
+++ b/Automationdashboard/MAIN_FOLDER/Automation_Dashboard_Batterywise/V4/D11_03_2024/merged_analysis.xlsx
@@ -432,47 +432,47 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>Value 1</t>
+          <t>analysis_B4_BT02_09.56_10.40.xlsx</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>Value 2</t>
+          <t>analysis_B4_BT02_13.59_14.50.xlsx</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>Value 3</t>
+          <t>analysis_B4_BT03_14.54_15.49.xlsx</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>Value 4</t>
+          <t>analysis_B4_BT04_10.45_11.45.xlsx</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>Value 5</t>
+          <t>analysis_B4_BT04_15.52_16.57.xlsx</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>Value 6</t>
+          <t>analysis_B4_BT05_11.47_12.42.xlsx</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>Value 7</t>
+          <t>analysis_B4_BT06_09.00_09.55.xlsx</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>Value 8</t>
+          <t>analysis_B4_BT06_13.03_13.56.xlsx</t>
         </is>
       </c>
       <c r="J1" t="inlineStr">
         <is>
-          <t>Value 9</t>
+          <t>analysis_B4_BT06_17.05_17.45.xlsx</t>
         </is>
       </c>
     </row>

</xml_diff>